<commit_message>
annas update of translations
</commit_message>
<xml_diff>
--- a/translations/translationsGuestMail.xlsx
+++ b/translations/translationsGuestMail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\jguese\Code\bw-dwh-microk8s\customDockerImages\contactform\bw-contactformbackend\emailbuilderapp\src\bw-email-templates\translations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annafoltinek/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED2DC71-B9A2-4761-A54B-6485A9181A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B06227-3349-A04C-BF88-4328F6F9694D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="3820" windowWidth="28800" windowHeight="15460" xr2:uid="{DC24FCB6-CF4A-41A1-98A3-EBA8ADD28FD1}"/>
+    <workbookView xWindow="-19080" yWindow="-10420" windowWidth="19080" windowHeight="21600" xr2:uid="{DC24FCB6-CF4A-41A1-98A3-EBA8ADD28FD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="259">
   <si>
     <t>German</t>
   </si>
@@ -108,12 +108,6 @@
     <t>Ausgefüllt am</t>
   </si>
   <si>
-    <t>Completed on</t>
-  </si>
-  <si>
-    <t>Cumplimentado el</t>
-  </si>
-  <si>
     <t>Einverständniserklärung</t>
   </si>
   <si>
@@ -124,18 +118,6 @@
   </si>
   <si>
     <t>Déclaration de consentement</t>
-  </si>
-  <si>
-    <t>erteilte Zustimmung</t>
-  </si>
-  <si>
-    <t>Given consent</t>
-  </si>
-  <si>
-    <t>Autorización concedida</t>
-  </si>
-  <si>
-    <t>Autorisation accordée</t>
   </si>
   <si>
     <t>columnname</t>
@@ -275,9 +257,6 @@
     <t>info_consent</t>
   </si>
   <si>
-    <t>Dûment rempli, le</t>
-  </si>
-  <si>
     <t>Stimmt etwas nicht oder sollte geändert werden? Lassen Sie es uns über [email] wissen.</t>
   </si>
   <si>
@@ -299,21 +278,12 @@
     <t>info_birthday</t>
   </si>
   <si>
-    <t>Birthday</t>
-  </si>
-  <si>
     <t>info_placeofbirth</t>
   </si>
   <si>
-    <t>Place of birth</t>
-  </si>
-  <si>
     <t>info_job</t>
   </si>
   <si>
-    <t>Job</t>
-  </si>
-  <si>
     <t>info_nationality</t>
   </si>
   <si>
@@ -389,21 +359,12 @@
     <t>info_media</t>
   </si>
   <si>
-    <t>Media</t>
-  </si>
-  <si>
     <t>info_therapytype</t>
   </si>
   <si>
-    <t>Therapy Wish</t>
-  </si>
-  <si>
     <t>heading_healthinfo</t>
   </si>
   <si>
-    <t>Your health Information</t>
-  </si>
-  <si>
     <t>info_weight</t>
   </si>
   <si>
@@ -425,9 +386,6 @@
     <t>info_support</t>
   </si>
   <si>
-    <t>Support needed</t>
-  </si>
-  <si>
     <t>info_contra</t>
   </si>
   <si>
@@ -578,9 +536,6 @@
     <t>Telefon</t>
   </si>
   <si>
-    <t>Anderes Telefon</t>
-  </si>
-  <si>
     <t>Notfallkontakt</t>
   </si>
   <si>
@@ -596,12 +551,6 @@
     <t>Abreise</t>
   </si>
   <si>
-    <t>Medien</t>
-  </si>
-  <si>
-    <t>Therapiewunsch</t>
-  </si>
-  <si>
     <t>Ihre Gesundheitsinformation</t>
   </si>
   <si>
@@ -617,42 +566,24 @@
     <t>Unterstützung benötigt</t>
   </si>
   <si>
-    <t>Ausschließende Kriterien</t>
-  </si>
-  <si>
-    <t>Medikation</t>
-  </si>
-  <si>
     <t>Weitere Information</t>
   </si>
   <si>
-    <t>Empfohlen von</t>
-  </si>
-  <si>
     <t>Nombre</t>
   </si>
   <si>
     <t>Género</t>
   </si>
   <si>
-    <t>Cumpleaños</t>
-  </si>
-  <si>
     <t>Lugar de nacimiento</t>
   </si>
   <si>
-    <t>Trabajo</t>
-  </si>
-  <si>
     <t>Nacionalidad</t>
   </si>
   <si>
     <t>Idioma(s)</t>
   </si>
   <si>
-    <t>Su información de contacto</t>
-  </si>
-  <si>
     <t>Teléfono</t>
   </si>
   <si>
@@ -674,27 +605,12 @@
     <t>Salida</t>
   </si>
   <si>
-    <t>Medios</t>
-  </si>
-  <si>
-    <t>Deseo de terapia</t>
-  </si>
-  <si>
-    <t>Información sobre su salud</t>
-  </si>
-  <si>
-    <t>Peso</t>
-  </si>
-  <si>
     <t>Altura</t>
   </si>
   <si>
     <t>Alergias</t>
   </si>
   <si>
-    <t>Apoyo necesario</t>
-  </si>
-  <si>
     <t>Enfermedades contraindicadas</t>
   </si>
   <si>
@@ -710,27 +626,12 @@
     <t>Nom</t>
   </si>
   <si>
-    <t>Genre</t>
-  </si>
-  <si>
-    <t>Anniversaire</t>
-  </si>
-  <si>
-    <t>Place de naissance</t>
-  </si>
-  <si>
-    <t>Emploi</t>
-  </si>
-  <si>
     <t>Nationalité</t>
   </si>
   <si>
     <t>Langue(s)</t>
   </si>
   <si>
-    <t>Vos coordonnées</t>
-  </si>
-  <si>
     <t>Courriel</t>
   </si>
   <si>
@@ -755,24 +656,6 @@
     <t>Départ</t>
   </si>
   <si>
-    <t>Médias</t>
-  </si>
-  <si>
-    <t>Souhaits thérapeutiques</t>
-  </si>
-  <si>
-    <t>Vos informations de santé</t>
-  </si>
-  <si>
-    <t>Poids</t>
-  </si>
-  <si>
-    <t>Hauteur</t>
-  </si>
-  <si>
-    <t>Soutien nécessaire</t>
-  </si>
-  <si>
     <t>Maladies contre-indiquées</t>
   </si>
   <si>
@@ -801,6 +684,126 @@
   </si>
   <si>
     <t>{info_consent}</t>
+  </si>
+  <si>
+    <t>Sexe</t>
+  </si>
+  <si>
+    <t>Fecha de nacimiento</t>
+  </si>
+  <si>
+    <t>Date de naissance</t>
+  </si>
+  <si>
+    <t>Date of birth</t>
+  </si>
+  <si>
+    <t>Birthplace</t>
+  </si>
+  <si>
+    <t>Lieu de naissance</t>
+  </si>
+  <si>
+    <t>Beruf</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>Profession</t>
+  </si>
+  <si>
+    <t>Ocupacíon</t>
+  </si>
+  <si>
+    <t>Información de contacto</t>
+  </si>
+  <si>
+    <t>Informations de contact</t>
+  </si>
+  <si>
+    <t>Weitere Telefonnummer</t>
+  </si>
+  <si>
+    <t>Wish for TV</t>
+  </si>
+  <si>
+    <t>TV Wunsch</t>
+  </si>
+  <si>
+    <t>Deseo de televisión</t>
+  </si>
+  <si>
+    <t>Souhaits pour la télévision</t>
+  </si>
+  <si>
+    <t>Kontaktaufnahme  Therapieplanung</t>
+  </si>
+  <si>
+    <t>Contact by therapy planning</t>
+  </si>
+  <si>
+    <t>Contact par la planification de la thérapie</t>
+  </si>
+  <si>
+    <t>Contacto a través de la planificación de la terapia</t>
+  </si>
+  <si>
+    <t>Your health</t>
+  </si>
+  <si>
+    <t>Votre santé</t>
+  </si>
+  <si>
+    <t>Su salud</t>
+  </si>
+  <si>
+    <t>Peso corposal</t>
+  </si>
+  <si>
+    <t>Taille</t>
+  </si>
+  <si>
+    <t>Poids corporel</t>
+  </si>
+  <si>
+    <t>Soutien quotidien nécessaire</t>
+  </si>
+  <si>
+    <t>Apoyo diario necesario</t>
+  </si>
+  <si>
+    <t>Daily support needed</t>
+  </si>
+  <si>
+    <t>Kontraindikative Erkrankungen</t>
+  </si>
+  <si>
+    <t>Medikamente</t>
+  </si>
+  <si>
+    <t>Empfohlen durch</t>
+  </si>
+  <si>
+    <t>Given consent to</t>
+  </si>
+  <si>
+    <t>Zustimmung erteilt zu</t>
+  </si>
+  <si>
+    <t>Dado el consentimiento para</t>
+  </si>
+  <si>
+    <t>Consentement donné à</t>
+  </si>
+  <si>
+    <t>Filled out on</t>
+  </si>
+  <si>
+    <t>Rempli le</t>
+  </si>
+  <si>
+    <t>Rellenado en</t>
   </si>
 </sst>
 </file>
@@ -1236,26 +1239,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{324DCE6B-D8DA-4DAE-A3E1-5B96D18552E0}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" customWidth="1"/>
-    <col min="3" max="3" width="43.1796875" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" customWidth="1"/>
-    <col min="6" max="6" width="33.08984375" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" customWidth="1"/>
+    <col min="4" max="4" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1267,135 +1270,135 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="B5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="3" t="s">
+    <row r="6" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="87" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B5" t="s">
-        <v>253</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="3" t="s">
+    </row>
+    <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B6" t="s">
-        <v>254</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="174" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" t="s">
-        <v>255</v>
-      </c>
-      <c r="C7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>70</v>
-      </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>3</v>
@@ -1410,12 +1413,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -1430,12 +1433,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>11</v>
@@ -1450,29 +1453,29 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>256</v>
+        <v>217</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>15</v>
@@ -1487,12 +1490,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>19</v>
@@ -1507,12 +1510,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>22</v>
@@ -1527,641 +1530,641 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>256</v>
+      </c>
+      <c r="E15" t="s">
+        <v>258</v>
+      </c>
+      <c r="F15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s">
+        <v>218</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D17" t="s">
+        <v>252</v>
+      </c>
+      <c r="E17" t="s">
+        <v>254</v>
+      </c>
+      <c r="F17" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" t="s">
+        <v>180</v>
+      </c>
+      <c r="F19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>80</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" t="s">
+        <v>162</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" t="s">
+        <v>222</v>
+      </c>
+      <c r="E21" t="s">
+        <v>220</v>
+      </c>
+      <c r="F21" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" t="s">
+        <v>164</v>
+      </c>
+      <c r="D22" t="s">
+        <v>223</v>
+      </c>
+      <c r="E22" t="s">
+        <v>182</v>
+      </c>
+      <c r="F22" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" t="s">
+        <v>225</v>
+      </c>
+      <c r="D23" t="s">
+        <v>226</v>
+      </c>
+      <c r="E23" t="s">
+        <v>228</v>
+      </c>
+      <c r="F23" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" t="s">
+        <v>183</v>
+      </c>
+      <c r="F24" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F25" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" t="s">
+        <v>167</v>
+      </c>
+      <c r="D26" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" t="s">
+        <v>229</v>
+      </c>
+      <c r="F26" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" t="s">
+        <v>185</v>
+      </c>
+      <c r="F28" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" t="s">
-        <v>257</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C31" t="s">
+        <v>169</v>
+      </c>
+      <c r="D31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" t="s">
+        <v>187</v>
+      </c>
+      <c r="F31" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" t="s">
         <v>147</v>
       </c>
-      <c r="C18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C32" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" t="s">
+        <v>188</v>
+      </c>
+      <c r="F32" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
         <v>148</v>
       </c>
-      <c r="C19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" t="s">
-        <v>200</v>
-      </c>
-      <c r="F19" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C33" t="s">
+        <v>171</v>
+      </c>
+      <c r="D33" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" t="s">
+        <v>189</v>
+      </c>
+      <c r="F33" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" t="s">
         <v>149</v>
       </c>
-      <c r="C20" t="s">
-        <v>176</v>
-      </c>
-      <c r="D20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" t="s">
-        <v>201</v>
-      </c>
-      <c r="F20" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" t="s">
+        <v>190</v>
+      </c>
+      <c r="F34" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" t="s">
         <v>150</v>
       </c>
-      <c r="C21" t="s">
-        <v>177</v>
-      </c>
-      <c r="D21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" t="s">
-        <v>202</v>
-      </c>
-      <c r="F21" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C35" t="s">
+        <v>173</v>
+      </c>
+      <c r="D35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" t="s">
+        <v>191</v>
+      </c>
+      <c r="F35" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" t="s">
         <v>151</v>
       </c>
-      <c r="C22" t="s">
-        <v>178</v>
-      </c>
-      <c r="D22" t="s">
-        <v>92</v>
-      </c>
-      <c r="E22" t="s">
-        <v>203</v>
-      </c>
-      <c r="F22" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>93</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C36" t="s">
+        <v>233</v>
+      </c>
+      <c r="D36" t="s">
+        <v>232</v>
+      </c>
+      <c r="E36" t="s">
+        <v>234</v>
+      </c>
+      <c r="F36" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" t="s">
         <v>152</v>
       </c>
-      <c r="C23" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" t="s">
-        <v>204</v>
-      </c>
-      <c r="F23" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>95</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="C37" t="s">
+        <v>236</v>
+      </c>
+      <c r="D37" t="s">
+        <v>237</v>
+      </c>
+      <c r="E37" t="s">
+        <v>239</v>
+      </c>
+      <c r="F37" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" t="s">
+        <v>174</v>
+      </c>
+      <c r="D38" t="s">
+        <v>240</v>
+      </c>
+      <c r="E38" t="s">
+        <v>242</v>
+      </c>
+      <c r="F38" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" t="s">
         <v>153</v>
       </c>
-      <c r="C24" t="s">
-        <v>179</v>
-      </c>
-      <c r="D24" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" t="s">
-        <v>205</v>
-      </c>
-      <c r="F24" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" t="s">
-        <v>154</v>
-      </c>
-      <c r="C25" t="s">
-        <v>180</v>
-      </c>
-      <c r="D25" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" t="s">
-        <v>206</v>
-      </c>
-      <c r="F25" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" t="s">
-        <v>155</v>
-      </c>
-      <c r="C26" t="s">
-        <v>181</v>
-      </c>
-      <c r="D26" t="s">
-        <v>100</v>
-      </c>
-      <c r="E26" t="s">
-        <v>207</v>
-      </c>
-      <c r="F26" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>101</v>
-      </c>
-      <c r="B27" t="s">
-        <v>156</v>
-      </c>
-      <c r="C27" t="s">
-        <v>102</v>
-      </c>
-      <c r="D27" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" t="s">
-        <v>102</v>
-      </c>
-      <c r="F27" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>103</v>
-      </c>
-      <c r="B28" t="s">
-        <v>157</v>
-      </c>
-      <c r="C28" t="s">
-        <v>182</v>
-      </c>
-      <c r="D28" t="s">
-        <v>104</v>
-      </c>
-      <c r="E28" t="s">
-        <v>208</v>
-      </c>
-      <c r="F28" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>105</v>
-      </c>
-      <c r="B29" t="s">
-        <v>158</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" t="s">
-        <v>159</v>
-      </c>
-      <c r="C30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E30" t="s">
-        <v>108</v>
-      </c>
-      <c r="F30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>109</v>
-      </c>
-      <c r="B31" t="s">
-        <v>160</v>
-      </c>
-      <c r="C31" t="s">
-        <v>184</v>
-      </c>
-      <c r="D31" t="s">
-        <v>110</v>
-      </c>
-      <c r="E31" t="s">
-        <v>210</v>
-      </c>
-      <c r="F31" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>111</v>
-      </c>
-      <c r="B32" t="s">
-        <v>161</v>
-      </c>
-      <c r="C32" t="s">
-        <v>185</v>
-      </c>
-      <c r="D32" t="s">
-        <v>112</v>
-      </c>
-      <c r="E32" t="s">
-        <v>211</v>
-      </c>
-      <c r="F32" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="C39" t="s">
+        <v>175</v>
+      </c>
+      <c r="D39" t="s">
         <v>113</v>
       </c>
-      <c r="B33" t="s">
-        <v>162</v>
-      </c>
-      <c r="C33" t="s">
-        <v>186</v>
-      </c>
-      <c r="D33" t="s">
-        <v>114</v>
-      </c>
-      <c r="E33" t="s">
-        <v>212</v>
-      </c>
-      <c r="F33" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>115</v>
-      </c>
-      <c r="B34" t="s">
-        <v>163</v>
-      </c>
-      <c r="C34" t="s">
-        <v>187</v>
-      </c>
-      <c r="D34" t="s">
-        <v>116</v>
-      </c>
-      <c r="E34" t="s">
-        <v>213</v>
-      </c>
-      <c r="F34" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>117</v>
-      </c>
-      <c r="B35" t="s">
-        <v>164</v>
-      </c>
-      <c r="C35" t="s">
-        <v>188</v>
-      </c>
-      <c r="D35" t="s">
-        <v>118</v>
-      </c>
-      <c r="E35" t="s">
-        <v>214</v>
-      </c>
-      <c r="F35" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>119</v>
-      </c>
-      <c r="B36" t="s">
-        <v>165</v>
-      </c>
-      <c r="C36" t="s">
-        <v>189</v>
-      </c>
-      <c r="D36" t="s">
-        <v>120</v>
-      </c>
-      <c r="E36" t="s">
-        <v>215</v>
-      </c>
-      <c r="F36" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>121</v>
-      </c>
-      <c r="B37" t="s">
-        <v>166</v>
-      </c>
-      <c r="C37" t="s">
-        <v>190</v>
-      </c>
-      <c r="D37" t="s">
-        <v>122</v>
-      </c>
-      <c r="E37" t="s">
-        <v>216</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="E39" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>123</v>
-      </c>
-      <c r="B38" t="s">
-        <v>175</v>
-      </c>
-      <c r="C38" t="s">
-        <v>191</v>
-      </c>
-      <c r="D38" t="s">
-        <v>124</v>
-      </c>
-      <c r="E38" t="s">
-        <v>217</v>
-      </c>
-      <c r="F38" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" t="s">
-        <v>167</v>
-      </c>
-      <c r="C39" t="s">
-        <v>192</v>
-      </c>
-      <c r="D39" t="s">
-        <v>126</v>
-      </c>
-      <c r="E39" t="s">
-        <v>218</v>
       </c>
       <c r="F39" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B40" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C40" t="s">
+        <v>176</v>
+      </c>
+      <c r="D40" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40" t="s">
+        <v>192</v>
+      </c>
+      <c r="F40" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" t="s">
+        <v>177</v>
+      </c>
+      <c r="D41" t="s">
+        <v>117</v>
+      </c>
+      <c r="E41" t="s">
         <v>193</v>
       </c>
-      <c r="D40" t="s">
-        <v>128</v>
-      </c>
-      <c r="E40" t="s">
-        <v>219</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="F41" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D42" t="s">
+        <v>248</v>
+      </c>
+      <c r="E42" t="s">
+        <v>247</v>
+      </c>
+      <c r="F42" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>129</v>
-      </c>
-      <c r="B41" t="s">
-        <v>169</v>
-      </c>
-      <c r="C41" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B43" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" t="s">
+        <v>249</v>
+      </c>
+      <c r="D43" t="s">
+        <v>120</v>
+      </c>
+      <c r="E43" t="s">
         <v>194</v>
       </c>
-      <c r="D41" t="s">
-        <v>130</v>
-      </c>
-      <c r="E41" t="s">
-        <v>220</v>
-      </c>
-      <c r="F41" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>131</v>
-      </c>
-      <c r="B42" t="s">
-        <v>170</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="F43" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" t="s">
+        <v>158</v>
+      </c>
+      <c r="C44" t="s">
+        <v>250</v>
+      </c>
+      <c r="D44" t="s">
+        <v>122</v>
+      </c>
+      <c r="E44" t="s">
         <v>195</v>
       </c>
-      <c r="D42" t="s">
-        <v>132</v>
-      </c>
-      <c r="E42" t="s">
-        <v>221</v>
-      </c>
-      <c r="F42" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>133</v>
-      </c>
-      <c r="B43" t="s">
-        <v>171</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="F44" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45" t="s">
+        <v>159</v>
+      </c>
+      <c r="C45" t="s">
+        <v>179</v>
+      </c>
+      <c r="D45" t="s">
+        <v>124</v>
+      </c>
+      <c r="E45" t="s">
         <v>196</v>
       </c>
-      <c r="D43" t="s">
-        <v>134</v>
-      </c>
-      <c r="E43" t="s">
-        <v>222</v>
-      </c>
-      <c r="F43" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>135</v>
-      </c>
-      <c r="B44" t="s">
-        <v>172</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="F45" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" t="s">
+        <v>160</v>
+      </c>
+      <c r="C46" t="s">
+        <v>251</v>
+      </c>
+      <c r="D46" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46" t="s">
         <v>197</v>
       </c>
-      <c r="D44" t="s">
-        <v>136</v>
-      </c>
-      <c r="E44" t="s">
-        <v>223</v>
-      </c>
-      <c r="F44" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>137</v>
-      </c>
-      <c r="B45" t="s">
-        <v>173</v>
-      </c>
-      <c r="C45" t="s">
-        <v>198</v>
-      </c>
-      <c r="D45" t="s">
-        <v>138</v>
-      </c>
-      <c r="E45" t="s">
-        <v>224</v>
-      </c>
-      <c r="F45" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>139</v>
-      </c>
-      <c r="B46" t="s">
-        <v>174</v>
-      </c>
-      <c r="C46" t="s">
-        <v>199</v>
-      </c>
-      <c r="D46" t="s">
-        <v>140</v>
-      </c>
-      <c r="E46" t="s">
-        <v>225</v>
-      </c>
       <c r="F46" t="s">
-        <v>251</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>